<commit_message>
Novos arquivos do Back end
</commit_message>
<xml_diff>
--- a/TrendsDiaria.xlsx
+++ b/TrendsDiaria.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{70944C74-D841-8B4C-8160-FA1BE1E42F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{781504BA-3E5D-114D-A462-69F14A47E6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="27">
   <si>
     <t>Quantidade de vídeos</t>
   </si>
@@ -41,46 +41,31 @@
     <t>Hashtag</t>
   </si>
   <si>
-    <t>#nofap</t>
-  </si>
-  <si>
-    <t>Caraca o nofap ksks</t>
-  </si>
-  <si>
-    <t>Nofap September</t>
-  </si>
-  <si>
-    <t>#FalandoMalPelasCostas</t>
-  </si>
-  <si>
-    <t>E gostou da vista?</t>
-  </si>
-  <si>
-    <t>Baixaria</t>
-  </si>
-  <si>
-    <t>#codelife</t>
-  </si>
-  <si>
-    <t>Minha vida dev</t>
-  </si>
-  <si>
-    <t>Vida de programador</t>
-  </si>
-  <si>
-    <t>#coreanoba</t>
-  </si>
-  <si>
-    <t>Coreano na Bahia</t>
-  </si>
-  <si>
-    <t>#praia</t>
-  </si>
-  <si>
-    <t>Foto na praia</t>
-  </si>
-  <si>
-    <t>Foto em uma praia</t>
+    <t>#borabill</t>
+  </si>
+  <si>
+    <t>Bora Biil</t>
+  </si>
+  <si>
+    <t>Dança da música Bora Bill</t>
+  </si>
+  <si>
+    <t>#elizabeth</t>
+  </si>
+  <si>
+    <t>Pensava que era imortal</t>
+  </si>
+  <si>
+    <t>Vídeo com narração chorando por que pensava que a Rainha Elizabeth era imortal</t>
+  </si>
+  <si>
+    <t>#sonho</t>
+  </si>
+  <si>
+    <t>Pensava que era realidad3</t>
+  </si>
+  <si>
+    <t>Finge que ta sonhando que ganhou milhões de reais e acorda com gritos da mãe</t>
   </si>
 </sst>
 </file>
@@ -447,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E8801D-274B-7B4A-B906-30EEDC652F6A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -483,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>60000</v>
+        <v>4000</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -497,7 +482,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>104000</v>
+        <v>7000</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -511,38 +496,10 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>208</v>
+        <v>9000</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>30000</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>70000</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>